<commit_message>
Began creating assessment classes
</commit_message>
<xml_diff>
--- a/Classes.xlsx
+++ b/Classes.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Documents\AssessmentManager\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Exam</t>
   </si>
@@ -27,9 +32,6 @@
     <t>List&lt;Question&gt;</t>
   </si>
   <si>
-    <t>TimeCreated</t>
-  </si>
-  <si>
     <t>DateTime</t>
   </si>
   <si>
@@ -84,9 +86,6 @@
     <t>CourseTitle</t>
   </si>
   <si>
-    <t>ExamDescription</t>
-  </si>
-  <si>
     <t>QuestionIndex</t>
   </si>
   <si>
@@ -109,6 +108,15 @@
   </si>
   <si>
     <t>ExaminerComment</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>AssessmentDescription</t>
+  </si>
+  <si>
+    <t>DateCreated</t>
   </si>
 </sst>
 </file>
@@ -175,6 +183,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -222,7 +233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,7 +268,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,31 +480,31 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -501,129 +512,129 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="H8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -631,21 +642,21 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +671,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -672,7 +683,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>